<commit_message>
Add scripts for switching PowerShell versions and syncing organizational group properties in SharePoint Online
</commit_message>
<xml_diff>
--- a/Entra/User Lifecycle/Bulk onboarding PS Graph SDK/Create New User.xlsx
+++ b/Entra/User Lifecycle/Bulk onboarding PS Graph SDK/Create New User.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mhud-my.sharepoint.com/personal/ashley_forde_hud_govt_nz/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HUD\Git_Repositories\Microsoft-365-and-Azure\Entra\User Lifecycle\Bulk onboarding PS Graph SDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="8_{03B301D7-57C6-4E57-BB21-8C81B8923B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2F95742-6528-4332-B5D2-0EA5CDEFD204}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FA211A-A887-42DF-A27B-9C7233ABFC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="27690" windowHeight="16560" xr2:uid="{EC62C7F1-0864-4F6C-8D7F-6E3A57BB67E6}"/>
+    <workbookView xWindow="15645" yWindow="4335" windowWidth="38700" windowHeight="15345" xr2:uid="{EC62C7F1-0864-4F6C-8D7F-6E3A57BB67E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>First Name</t>
   </si>
@@ -172,43 +172,25 @@
     <t>Level 9,7 Waterloo Quay,Pipitea,Wellington</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Test Engineer</t>
-  </si>
-  <si>
-    <t>Digital</t>
-  </si>
-  <si>
-    <t>Organisational Performance</t>
-  </si>
-  <si>
-    <t>Test User 2</t>
-  </si>
-  <si>
-    <t>Test User 3</t>
-  </si>
-  <si>
-    <t>User 2</t>
-  </si>
-  <si>
-    <t>User 3</t>
-  </si>
-  <si>
-    <t>Ashley.Forde@hud.govt.nz</t>
-  </si>
-  <si>
-    <t>Janine.Crous@hud.govt.nz</t>
-  </si>
-  <si>
-    <t>Devon.Heaphy@hud.govt.nz</t>
-  </si>
-  <si>
-    <t>User 1</t>
-  </si>
-  <si>
-    <t>Test User 1</t>
+    <t>Isabella</t>
+  </si>
+  <si>
+    <t>DaggCourt</t>
+  </si>
+  <si>
+    <t>Isabella Dagg Court</t>
+  </si>
+  <si>
+    <t>Policy Advisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operational Policy </t>
+  </si>
+  <si>
+    <t>Policy</t>
+  </si>
+  <si>
+    <t>Rebekah.Hood@hud.govt.nz</t>
   </si>
 </sst>
 </file>
@@ -274,9 +256,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -314,7 +296,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -420,7 +402,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -562,7 +544,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -573,7 +555,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -635,118 +617,45 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="str" cm="1">
-        <f t="array" ref="H2">IF(G2="Auckland", AucklandAddresses, IF(G2="Wellington", WellingtonAddresses, ""))</f>
-        <v>Level 7, 45 Queen Street, Auckland</v>
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(J2), "", IFERROR(VLOOKUP(J2, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v>ORA_HRX_CONSULTANT</v>
+        <v>HUD_SUBSTANTIVE_POSITION</v>
       </c>
       <c r="L2" s="2">
-        <v>45373</v>
+        <v>45670</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="str">
-        <f>IF(ISBLANK(J3), "", IFERROR(VLOOKUP(J3, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v>HUD_FIX_TERM</v>
-      </c>
-      <c r="L3" s="2">
-        <v>45374</v>
-      </c>
+      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="str">
-        <f>IF(ISBLANK(J4), "", IFERROR(VLOOKUP(J4, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v>HUD_SUBSTANTIVE_POSITION</v>
-      </c>
-      <c r="L4" s="2">
-        <v>45375</v>
-      </c>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K5" t="str">

</xml_diff>